<commit_message>
added emergent theory diagram, edited timetable to add more interviews, edited interview questions because for some reason the pdf hadn't changed
</commit_message>
<xml_diff>
--- a/TIMETABLE_LAST_WEEKS.xlsx
+++ b/TIMETABLE_LAST_WEEKS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lavanyasajwan/Documents/University/2020/engr489/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59A726CD-038A-194E-9605-FF74AFA3F01F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF85AF3-EF6A-8D4C-9F98-59EBF06F6917}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="41">
   <si>
     <t>Daily Schedule</t>
   </si>
@@ -100,9 +100,6 @@
     <t>DIS CLASS</t>
   </si>
   <si>
-    <t>HCI MEETING</t>
-  </si>
-  <si>
     <t>DIS REPORT</t>
   </si>
   <si>
@@ -127,9 +124,6 @@
     <t>Mon (SWEN433 DUE)</t>
   </si>
   <si>
-    <t>SWEN423 MOCK TERMS TEST</t>
-  </si>
-  <si>
     <t>9/19/2020</t>
   </si>
   <si>
@@ -137,9 +131,6 @@
   </si>
   <si>
     <t>Thur (ENGR489 DUE TOMORROW)</t>
-  </si>
-  <si>
-    <t>Q</t>
   </si>
   <si>
     <t>Fri (DRAFT ENGR489 DUE+ SWEN423 MOCK TEST&amp;READINGS )</t>
@@ -158,6 +149,18 @@
   </si>
   <si>
     <t>VUWWIT AGM</t>
+  </si>
+  <si>
+    <t>DOCTOR'S APPOINTMENT</t>
+  </si>
+  <si>
+    <t>INTERVIEW</t>
+  </si>
+  <si>
+    <t>SUPERVISOR MEETING</t>
+  </si>
+  <si>
+    <t>SWEN433 REPORT</t>
   </si>
 </sst>
 </file>
@@ -245,7 +248,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -308,12 +311,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
@@ -327,6 +324,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -375,7 +390,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -464,9 +479,6 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -497,13 +509,28 @@
     <xf numFmtId="0" fontId="9" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1454,14 +1481,14 @@
   </sheetPr>
   <dimension ref="B1:AA52"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="F9" sqref="B5:I52"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F11" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="L26" sqref="K5:R52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="29" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="1.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="7.5" style="33" customWidth="1"/>
+    <col min="2" max="2" width="7.5" style="32" customWidth="1"/>
     <col min="3" max="3" width="19.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.83203125" style="1" bestFit="1" customWidth="1"/>
@@ -1470,7 +1497,7 @@
     <col min="8" max="8" width="23.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.83203125" style="1" customWidth="1"/>
     <col min="10" max="10" width="2" style="1" customWidth="1"/>
-    <col min="11" max="11" width="8.6640625" style="33"/>
+    <col min="11" max="11" width="8.6640625" style="32"/>
     <col min="12" max="12" width="65" style="1" customWidth="1"/>
     <col min="13" max="13" width="19" style="1" customWidth="1"/>
     <col min="14" max="14" width="12.5" style="1" bestFit="1" customWidth="1"/>
@@ -1479,7 +1506,7 @@
     <col min="17" max="17" width="17" style="1" customWidth="1"/>
     <col min="18" max="18" width="15.5" style="1" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="2" style="1" customWidth="1"/>
-    <col min="20" max="20" width="8.6640625" style="33"/>
+    <col min="20" max="20" width="8.6640625" style="32"/>
     <col min="21" max="21" width="27.6640625" style="1" customWidth="1"/>
     <col min="22" max="22" width="9.5" style="1" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="10.5" style="1" customWidth="1"/>
@@ -1491,7 +1518,7 @@
   <sheetData>
     <row r="1" spans="2:27" ht="9" customHeight="1"/>
     <row r="2" spans="2:27" ht="33" customHeight="1">
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="33" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="3"/>
@@ -1502,7 +1529,7 @@
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
       <c r="J2" s="4"/>
-      <c r="K2" s="34" t="s">
+      <c r="K2" s="33" t="s">
         <v>0</v>
       </c>
       <c r="L2" s="3"/>
@@ -1512,7 +1539,7 @@
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
       <c r="R2" s="3"/>
-      <c r="T2" s="34" t="s">
+      <c r="T2" s="33" t="s">
         <v>0</v>
       </c>
       <c r="U2" s="3"/>
@@ -1524,7 +1551,7 @@
       <c r="AA2" s="3"/>
     </row>
     <row r="3" spans="2:27" ht="27.75" customHeight="1">
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="34" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="10">
@@ -1539,7 +1566,7 @@
       <c r="G3" s="6"/>
       <c r="H3" s="7"/>
       <c r="I3" s="2"/>
-      <c r="K3" s="35" t="s">
+      <c r="K3" s="34" t="s">
         <v>9</v>
       </c>
       <c r="L3" s="10">
@@ -1554,11 +1581,11 @@
       <c r="P3" s="6"/>
       <c r="Q3" s="7"/>
       <c r="R3" s="2"/>
-      <c r="T3" s="35" t="s">
+      <c r="T3" s="34" t="s">
         <v>9</v>
       </c>
       <c r="U3" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="W3" s="9" t="s">
         <v>8</v>
@@ -1571,7 +1598,7 @@
       <c r="AA3" s="2"/>
     </row>
     <row r="4" spans="2:27" ht="27" customHeight="1">
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="35" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="5" t="s">
@@ -1587,19 +1614,19 @@
         <v>1</v>
       </c>
       <c r="G4" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="5" t="s">
         <v>26</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>27</v>
       </c>
       <c r="I4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="36" t="s">
+      <c r="K4" s="35" t="s">
         <v>7</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="M4" s="5" t="s">
         <v>5</v>
@@ -1608,7 +1635,7 @@
         <v>6</v>
       </c>
       <c r="O4" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P4" s="5" t="s">
         <v>2</v>
@@ -1619,11 +1646,11 @@
       <c r="R4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="T4" s="36" t="s">
+      <c r="T4" s="35" t="s">
         <v>7</v>
       </c>
       <c r="U4" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="V4" s="5" t="s">
         <v>5</v>
@@ -1638,14 +1665,14 @@
         <v>2</v>
       </c>
       <c r="Z4" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="AA4" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="2:27" ht="29" customHeight="1">
-      <c r="B5" s="37">
+      <c r="B5" s="36">
         <f>StartTime</f>
         <v>0.29166666666666669</v>
       </c>
@@ -1656,7 +1683,7 @@
       <c r="G5" s="11"/>
       <c r="H5" s="11"/>
       <c r="I5" s="11"/>
-      <c r="K5" s="37">
+      <c r="K5" s="36">
         <f>StartTime</f>
         <v>0.29166666666666669</v>
       </c>
@@ -1667,7 +1694,7 @@
       <c r="P5" s="11"/>
       <c r="Q5" s="11"/>
       <c r="R5" s="11"/>
-      <c r="T5" s="37">
+      <c r="T5" s="36">
         <f>StartTime</f>
         <v>0.29166666666666669</v>
       </c>
@@ -1680,7 +1707,7 @@
       <c r="AA5" s="11"/>
     </row>
     <row r="6" spans="2:27" ht="29" customHeight="1">
-      <c r="B6" s="37">
+      <c r="B6" s="36">
         <f t="shared" ref="B6:B38" si="0">B5+TIME(0,30,0)</f>
         <v>0.3125</v>
       </c>
@@ -1691,7 +1718,7 @@
       <c r="G6" s="11"/>
       <c r="H6" s="11"/>
       <c r="I6" s="11"/>
-      <c r="K6" s="37">
+      <c r="K6" s="36">
         <f t="shared" ref="K6:K52" si="1">K5+TIME(0,30,0)</f>
         <v>0.3125</v>
       </c>
@@ -1702,7 +1729,7 @@
       <c r="P6" s="11"/>
       <c r="Q6" s="11"/>
       <c r="R6" s="11"/>
-      <c r="T6" s="37">
+      <c r="T6" s="36">
         <f t="shared" ref="T6:T52" si="2">T5+TIME(0,30,0)</f>
         <v>0.3125</v>
       </c>
@@ -1715,12 +1742,12 @@
       <c r="AA6" s="11"/>
     </row>
     <row r="7" spans="2:27" ht="29" customHeight="1">
-      <c r="B7" s="37">
+      <c r="B7" s="36">
         <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
@@ -1728,22 +1755,22 @@
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
       <c r="I7" s="11"/>
-      <c r="K7" s="37">
+      <c r="K7" s="36">
         <f t="shared" si="1"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="L7" s="38"/>
+      <c r="L7" s="37"/>
       <c r="M7" s="11"/>
       <c r="N7" s="11"/>
       <c r="O7" s="11"/>
       <c r="P7" s="11"/>
       <c r="Q7" s="11"/>
       <c r="R7" s="11"/>
-      <c r="T7" s="37">
+      <c r="T7" s="36">
         <f t="shared" si="2"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="U7" s="38"/>
+      <c r="U7" s="37"/>
       <c r="V7" s="11"/>
       <c r="W7" s="11"/>
       <c r="X7" s="11"/>
@@ -1752,12 +1779,12 @@
       <c r="AA7" s="11"/>
     </row>
     <row r="8" spans="2:27" ht="29" customHeight="1">
-      <c r="B8" s="37">
+      <c r="B8" s="36">
         <f t="shared" si="0"/>
         <v>0.35416666666666663</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
@@ -1765,25 +1792,25 @@
       <c r="G8" s="11"/>
       <c r="H8" s="11"/>
       <c r="I8" s="11"/>
-      <c r="K8" s="37">
+      <c r="K8" s="36">
         <f t="shared" si="1"/>
         <v>0.35416666666666663</v>
       </c>
-      <c r="L8" s="38"/>
+      <c r="L8" s="37"/>
       <c r="M8" s="11"/>
       <c r="N8" s="11"/>
       <c r="O8" s="11"/>
       <c r="P8" s="11"/>
       <c r="Q8" s="11"/>
       <c r="R8" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="T8" s="37">
+        <v>34</v>
+      </c>
+      <c r="T8" s="36">
         <f t="shared" si="2"/>
         <v>0.35416666666666663</v>
       </c>
       <c r="U8" s="16" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="V8" s="11"/>
       <c r="W8" s="11"/>
@@ -1793,152 +1820,150 @@
       <c r="AA8" s="19"/>
     </row>
     <row r="9" spans="2:27" ht="29" customHeight="1">
-      <c r="B9" s="37">
+      <c r="B9" s="36">
         <f t="shared" si="0"/>
         <v>0.37499999999999994</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D9" s="23" t="s">
         <v>13</v>
       </c>
       <c r="E9" s="22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F9" s="22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G9" s="22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H9" s="14"/>
       <c r="I9" s="11"/>
-      <c r="K9" s="37">
+      <c r="K9" s="36">
         <f t="shared" si="1"/>
         <v>0.37499999999999994</v>
       </c>
-      <c r="L9" s="20" t="s">
-        <v>16</v>
-      </c>
+      <c r="L9" s="47"/>
       <c r="M9" s="24"/>
       <c r="N9" s="24"/>
-      <c r="O9" s="39"/>
-      <c r="P9" s="39"/>
-      <c r="Q9" s="39"/>
+      <c r="O9" s="38"/>
+      <c r="P9" s="38"/>
+      <c r="Q9" s="38"/>
       <c r="R9" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="T9" s="37">
+        <v>34</v>
+      </c>
+      <c r="T9" s="36">
         <f t="shared" si="2"/>
         <v>0.37499999999999994</v>
       </c>
       <c r="U9" s="16" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="V9" s="24"/>
       <c r="W9" s="24"/>
-      <c r="X9" s="39"/>
-      <c r="Y9" s="39"/>
-      <c r="Z9" s="39"/>
+      <c r="X9" s="38"/>
+      <c r="Y9" s="38"/>
+      <c r="Z9" s="38"/>
       <c r="AA9" s="19"/>
     </row>
     <row r="10" spans="2:27" ht="29" customHeight="1">
-      <c r="B10" s="37">
+      <c r="B10" s="36">
         <f t="shared" si="0"/>
         <v>0.39583333333333326</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D10" s="23" t="s">
         <v>13</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F10" s="22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G10" s="22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H10" s="14"/>
       <c r="I10" s="11"/>
-      <c r="K10" s="37">
+      <c r="K10" s="36">
         <f t="shared" si="1"/>
         <v>0.39583333333333326</v>
       </c>
-      <c r="L10" s="20" t="s">
-        <v>16</v>
+      <c r="L10" s="43" t="s">
+        <v>37</v>
       </c>
       <c r="M10" s="24"/>
       <c r="N10" s="24"/>
-      <c r="O10" s="39"/>
-      <c r="P10" s="39"/>
-      <c r="Q10" s="39"/>
+      <c r="O10" s="38"/>
+      <c r="P10" s="38"/>
+      <c r="Q10" s="38"/>
       <c r="R10" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="T10" s="37">
+        <v>34</v>
+      </c>
+      <c r="T10" s="36">
         <f t="shared" si="2"/>
         <v>0.39583333333333326</v>
       </c>
       <c r="U10" s="16" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="V10" s="24"/>
       <c r="W10" s="24"/>
-      <c r="X10" s="39"/>
-      <c r="Y10" s="39"/>
-      <c r="Z10" s="39"/>
+      <c r="X10" s="38"/>
+      <c r="Y10" s="38"/>
+      <c r="Z10" s="38"/>
       <c r="AA10" s="20" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="11" spans="2:27" ht="29.5" customHeight="1">
-      <c r="B11" s="37">
+      <c r="B11" s="36">
         <f t="shared" si="0"/>
         <v>0.41666666666666657</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D11" s="26"/>
       <c r="E11" s="22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F11" s="22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G11" s="22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H11" s="14"/>
       <c r="I11" s="11"/>
-      <c r="K11" s="37">
+      <c r="K11" s="36">
         <f t="shared" si="1"/>
         <v>0.41666666666666657</v>
       </c>
       <c r="L11" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="M11" s="20" t="s">
-        <v>16</v>
+      <c r="M11" s="22" t="s">
+        <v>20</v>
       </c>
       <c r="N11" s="24"/>
-      <c r="O11" s="39"/>
-      <c r="P11" s="39"/>
-      <c r="Q11" s="39"/>
+      <c r="O11" s="38"/>
+      <c r="P11" s="38"/>
+      <c r="Q11" s="38"/>
       <c r="R11" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="T11" s="37">
+        <v>34</v>
+      </c>
+      <c r="T11" s="36">
         <f t="shared" si="2"/>
         <v>0.41666666666666657</v>
       </c>
       <c r="U11" s="16" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="V11" s="20" t="s">
         <v>16</v>
@@ -1960,34 +1985,34 @@
       </c>
     </row>
     <row r="12" spans="2:27" ht="29" customHeight="1">
-      <c r="B12" s="37">
+      <c r="B12" s="36">
         <f t="shared" si="0"/>
         <v>0.43749999999999989</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D12" s="26"/>
       <c r="E12" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="F12" s="31" t="s">
-        <v>22</v>
-      </c>
       <c r="G12" s="22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H12" s="14"/>
       <c r="I12" s="11"/>
-      <c r="K12" s="37">
+      <c r="K12" s="36">
         <f t="shared" si="1"/>
         <v>0.43749999999999989</v>
       </c>
       <c r="L12" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="M12" s="20" t="s">
-        <v>16</v>
+      <c r="M12" s="22" t="s">
+        <v>20</v>
       </c>
       <c r="N12" s="20" t="s">
         <v>16</v>
@@ -2002,14 +2027,14 @@
         <v>16</v>
       </c>
       <c r="R12" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="T12" s="37">
+        <v>34</v>
+      </c>
+      <c r="T12" s="36">
         <f t="shared" si="2"/>
         <v>0.43749999999999989</v>
       </c>
       <c r="U12" s="16" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="V12" s="20" t="s">
         <v>16</v>
@@ -2031,34 +2056,34 @@
       </c>
     </row>
     <row r="13" spans="2:27" ht="29" customHeight="1">
-      <c r="B13" s="37">
+      <c r="B13" s="36">
         <f t="shared" si="0"/>
         <v>0.4583333333333332</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D13" s="26"/>
       <c r="E13" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="F13" s="31" t="s">
-        <v>22</v>
-      </c>
       <c r="G13" s="22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H13" s="11"/>
       <c r="I13" s="11"/>
-      <c r="K13" s="37">
+      <c r="K13" s="36">
         <f t="shared" si="1"/>
         <v>0.4583333333333332</v>
       </c>
-      <c r="L13" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="M13" s="20" t="s">
-        <v>16</v>
+      <c r="L13" s="44" t="s">
+        <v>38</v>
+      </c>
+      <c r="M13" s="22" t="s">
+        <v>20</v>
       </c>
       <c r="N13" s="20" t="s">
         <v>16</v>
@@ -2073,14 +2098,14 @@
         <v>16</v>
       </c>
       <c r="R13" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="T13" s="37">
+        <v>34</v>
+      </c>
+      <c r="T13" s="36">
         <f t="shared" si="2"/>
         <v>0.4583333333333332</v>
       </c>
       <c r="U13" s="16" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="V13" s="20" t="s">
         <v>16</v>
@@ -2102,12 +2127,12 @@
       </c>
     </row>
     <row r="14" spans="2:27" ht="29" customHeight="1">
-      <c r="B14" s="37">
+      <c r="B14" s="36">
         <f t="shared" si="0"/>
         <v>0.47916666666666652</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D14" s="26"/>
       <c r="E14" s="27"/>
@@ -2115,21 +2140,21 @@
         <v>12</v>
       </c>
       <c r="G14" s="22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H14" s="20" t="s">
         <v>16</v>
       </c>
       <c r="I14" s="11"/>
-      <c r="K14" s="37">
+      <c r="K14" s="36">
         <f t="shared" si="1"/>
         <v>0.47916666666666652</v>
       </c>
-      <c r="L14" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="M14" s="20" t="s">
-        <v>16</v>
+      <c r="L14" s="44" t="s">
+        <v>38</v>
+      </c>
+      <c r="M14" s="23" t="s">
+        <v>40</v>
       </c>
       <c r="N14" s="20" t="s">
         <v>16</v>
@@ -2144,14 +2169,14 @@
         <v>16</v>
       </c>
       <c r="R14" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="T14" s="37">
+        <v>34</v>
+      </c>
+      <c r="T14" s="36">
         <f t="shared" si="2"/>
         <v>0.47916666666666652</v>
       </c>
       <c r="U14" s="16" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="V14" s="20" t="s">
         <v>16</v>
@@ -2173,12 +2198,12 @@
       </c>
     </row>
     <row r="15" spans="2:27" ht="29" customHeight="1">
-      <c r="B15" s="37">
+      <c r="B15" s="36">
         <f t="shared" si="0"/>
         <v>0.49999999999999983</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D15" s="26"/>
       <c r="E15" s="28"/>
@@ -2186,21 +2211,21 @@
         <v>12</v>
       </c>
       <c r="G15" s="22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H15" s="20" t="s">
         <v>16</v>
       </c>
       <c r="I15" s="11"/>
-      <c r="K15" s="37">
+      <c r="K15" s="36">
         <f t="shared" si="1"/>
         <v>0.49999999999999983</v>
       </c>
-      <c r="L15" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="M15" s="20" t="s">
-        <v>16</v>
+      <c r="L15" s="44" t="s">
+        <v>38</v>
+      </c>
+      <c r="M15" s="23" t="s">
+        <v>40</v>
       </c>
       <c r="N15" s="20" t="s">
         <v>16</v>
@@ -2215,14 +2240,14 @@
         <v>16</v>
       </c>
       <c r="R15" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="T15" s="37">
+        <v>34</v>
+      </c>
+      <c r="T15" s="36">
         <f t="shared" si="2"/>
         <v>0.49999999999999983</v>
       </c>
       <c r="U15" s="16" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="V15" s="20" t="s">
         <v>16</v>
@@ -2244,32 +2269,32 @@
       </c>
     </row>
     <row r="16" spans="2:27" ht="29" customHeight="1">
-      <c r="B16" s="37">
+      <c r="B16" s="36">
         <f t="shared" si="0"/>
         <v>0.52083333333333315</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D16" s="26"/>
       <c r="E16" s="28"/>
       <c r="F16" s="11"/>
       <c r="G16" s="22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H16" s="20" t="s">
         <v>16</v>
       </c>
       <c r="I16" s="11"/>
-      <c r="K16" s="37">
+      <c r="K16" s="36">
         <f t="shared" si="1"/>
         <v>0.52083333333333315</v>
       </c>
-      <c r="L16" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="M16" s="20" t="s">
-        <v>16</v>
+      <c r="L16" s="44" t="s">
+        <v>38</v>
+      </c>
+      <c r="M16" s="23" t="s">
+        <v>40</v>
       </c>
       <c r="N16" s="20" t="s">
         <v>16</v>
@@ -2284,19 +2309,19 @@
         <v>16</v>
       </c>
       <c r="R16" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="T16" s="37">
+        <v>34</v>
+      </c>
+      <c r="T16" s="36">
         <f t="shared" si="2"/>
         <v>0.52083333333333315</v>
       </c>
       <c r="U16" s="16" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="V16" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="W16" s="32"/>
+      <c r="W16" s="31"/>
       <c r="X16" s="11"/>
       <c r="Y16" s="20" t="s">
         <v>16</v>
@@ -2309,32 +2334,32 @@
       </c>
     </row>
     <row r="17" spans="2:27" ht="29" customHeight="1">
-      <c r="B17" s="37">
+      <c r="B17" s="36">
         <f t="shared" si="0"/>
         <v>0.54166666666666652</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D17" s="26"/>
       <c r="E17" s="28"/>
-      <c r="F17" s="31" t="s">
-        <v>22</v>
+      <c r="F17" s="30" t="s">
+        <v>21</v>
       </c>
       <c r="G17" s="24"/>
       <c r="H17" s="20" t="s">
         <v>16</v>
       </c>
       <c r="I17" s="11"/>
-      <c r="K17" s="37">
+      <c r="K17" s="36">
         <f t="shared" si="1"/>
         <v>0.54166666666666652</v>
       </c>
-      <c r="L17" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="M17" s="20" t="s">
-        <v>16</v>
+      <c r="L17" s="44" t="s">
+        <v>38</v>
+      </c>
+      <c r="M17" s="23" t="s">
+        <v>40</v>
       </c>
       <c r="N17" s="20" t="s">
         <v>16</v>
@@ -2349,19 +2374,19 @@
         <v>16</v>
       </c>
       <c r="R17" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="T17" s="37">
+        <v>34</v>
+      </c>
+      <c r="T17" s="36">
         <f t="shared" si="2"/>
         <v>0.54166666666666652</v>
       </c>
       <c r="U17" s="16" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="V17" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="W17" s="32"/>
+      <c r="W17" s="31"/>
       <c r="X17" s="22" t="s">
         <v>19</v>
       </c>
@@ -2376,28 +2401,26 @@
       </c>
     </row>
     <row r="18" spans="2:27" ht="29" customHeight="1">
-      <c r="B18" s="37">
+      <c r="B18" s="36">
         <f t="shared" si="0"/>
         <v>0.56249999999999989</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D18" s="26"/>
       <c r="E18" s="28"/>
-      <c r="F18" s="31" t="s">
-        <v>22</v>
+      <c r="F18" s="30" t="s">
+        <v>21</v>
       </c>
       <c r="G18" s="24"/>
       <c r="H18" s="11"/>
       <c r="I18" s="11"/>
-      <c r="K18" s="37">
+      <c r="K18" s="36">
         <f t="shared" si="1"/>
         <v>0.56249999999999989</v>
       </c>
-      <c r="L18" s="16" t="s">
-        <v>29</v>
-      </c>
+      <c r="L18" s="21"/>
       <c r="M18" s="25"/>
       <c r="N18" s="20" t="s">
         <v>16</v>
@@ -2412,19 +2435,19 @@
         <v>16</v>
       </c>
       <c r="R18" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="T18" s="37">
+        <v>34</v>
+      </c>
+      <c r="T18" s="36">
         <f t="shared" si="2"/>
         <v>0.56249999999999989</v>
       </c>
       <c r="U18" s="16" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="V18" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="W18" s="32"/>
+      <c r="W18" s="31"/>
       <c r="X18" s="22" t="s">
         <v>19</v>
       </c>
@@ -2439,7 +2462,7 @@
       </c>
     </row>
     <row r="19" spans="2:27" ht="29" customHeight="1">
-      <c r="B19" s="37">
+      <c r="B19" s="36">
         <f t="shared" si="0"/>
         <v>0.58333333333333326</v>
       </c>
@@ -2448,20 +2471,20 @@
       </c>
       <c r="D19" s="26"/>
       <c r="E19" s="29"/>
-      <c r="F19" s="31" t="s">
-        <v>22</v>
+      <c r="F19" s="30" t="s">
+        <v>21</v>
       </c>
       <c r="G19" s="24"/>
       <c r="H19" s="11"/>
-      <c r="I19" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="K19" s="37">
+      <c r="I19" s="45" t="s">
+        <v>21</v>
+      </c>
+      <c r="K19" s="36">
         <f t="shared" si="1"/>
         <v>0.58333333333333326</v>
       </c>
-      <c r="L19" s="24" t="s">
-        <v>33</v>
+      <c r="L19" s="46" t="s">
+        <v>39</v>
       </c>
       <c r="M19" s="25"/>
       <c r="N19" s="29"/>
@@ -2469,12 +2492,12 @@
       <c r="P19" s="11"/>
       <c r="Q19" s="11"/>
       <c r="R19" s="24"/>
-      <c r="T19" s="37">
+      <c r="T19" s="36">
         <f t="shared" si="2"/>
         <v>0.58333333333333326</v>
       </c>
       <c r="U19" s="16" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="V19" s="20" t="s">
         <v>16</v>
@@ -2492,7 +2515,7 @@
       </c>
     </row>
     <row r="20" spans="2:27" ht="29" customHeight="1">
-      <c r="B20" s="37">
+      <c r="B20" s="36">
         <f t="shared" si="0"/>
         <v>0.60416666666666663</v>
       </c>
@@ -2504,15 +2527,15 @@
       <c r="F20" s="24"/>
       <c r="G20" s="11"/>
       <c r="H20" s="11"/>
-      <c r="I20" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="K20" s="37">
+      <c r="I20" s="45" t="s">
+        <v>21</v>
+      </c>
+      <c r="K20" s="36">
         <f t="shared" si="1"/>
         <v>0.60416666666666663</v>
       </c>
-      <c r="L20" s="16" t="s">
-        <v>29</v>
+      <c r="L20" s="46" t="s">
+        <v>39</v>
       </c>
       <c r="M20" s="20" t="s">
         <v>16</v>
@@ -2522,12 +2545,12 @@
       <c r="P20" s="11"/>
       <c r="Q20" s="11"/>
       <c r="R20" s="24"/>
-      <c r="T20" s="37">
+      <c r="T20" s="36">
         <f t="shared" si="2"/>
         <v>0.60416666666666663</v>
       </c>
       <c r="U20" s="16" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="V20" s="20" t="s">
         <v>16</v>
@@ -2540,10 +2563,10 @@
       <c r="Z20" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="AA20" s="39"/>
+      <c r="AA20" s="38"/>
     </row>
     <row r="21" spans="2:27" ht="29" customHeight="1">
-      <c r="B21" s="37">
+      <c r="B21" s="36">
         <f t="shared" si="0"/>
         <v>0.625</v>
       </c>
@@ -2562,12 +2585,12 @@
       <c r="I21" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="K21" s="37">
+      <c r="K21" s="36">
         <f t="shared" si="1"/>
         <v>0.625</v>
       </c>
-      <c r="L21" s="16" t="s">
-        <v>29</v>
+      <c r="L21" s="46" t="s">
+        <v>39</v>
       </c>
       <c r="M21" s="20" t="s">
         <v>16</v>
@@ -2583,12 +2606,12 @@
       <c r="R21" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="T21" s="37">
+      <c r="T21" s="36">
         <f t="shared" si="2"/>
         <v>0.625</v>
       </c>
       <c r="U21" s="16" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="V21" s="20" t="s">
         <v>16</v>
@@ -2608,7 +2631,7 @@
       </c>
     </row>
     <row r="22" spans="2:27" ht="29" customHeight="1">
-      <c r="B22" s="37">
+      <c r="B22" s="36">
         <f t="shared" si="0"/>
         <v>0.64583333333333337</v>
       </c>
@@ -2629,12 +2652,12 @@
       <c r="I22" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="K22" s="37">
+      <c r="K22" s="36">
         <f t="shared" si="1"/>
         <v>0.64583333333333337</v>
       </c>
-      <c r="L22" s="16" t="s">
-        <v>29</v>
+      <c r="L22" s="46" t="s">
+        <v>39</v>
       </c>
       <c r="M22" s="20" t="s">
         <v>16</v>
@@ -2650,12 +2673,12 @@
       <c r="R22" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="T22" s="37">
+      <c r="T22" s="36">
         <f t="shared" si="2"/>
         <v>0.64583333333333337</v>
       </c>
       <c r="U22" s="16" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="V22" s="20" t="s">
         <v>16</v>
@@ -2675,7 +2698,7 @@
       </c>
     </row>
     <row r="23" spans="2:27" ht="29" customHeight="1">
-      <c r="B23" s="37">
+      <c r="B23" s="36">
         <f t="shared" si="0"/>
         <v>0.66666666666666674</v>
       </c>
@@ -2692,12 +2715,12 @@
         <v>16</v>
       </c>
       <c r="I23" s="11"/>
-      <c r="K23" s="37">
+      <c r="K23" s="36">
         <f t="shared" si="1"/>
         <v>0.66666666666666674</v>
       </c>
-      <c r="L23" s="16" t="s">
-        <v>29</v>
+      <c r="L23" s="20" t="s">
+        <v>16</v>
       </c>
       <c r="M23" s="20" t="s">
         <v>16</v>
@@ -2709,11 +2732,11 @@
         <v>16</v>
       </c>
       <c r="R23" s="11"/>
-      <c r="T23" s="37">
+      <c r="T23" s="36">
         <f t="shared" si="2"/>
         <v>0.66666666666666674</v>
       </c>
-      <c r="U23" s="39"/>
+      <c r="U23" s="38"/>
       <c r="V23" s="20" t="s">
         <v>16</v>
       </c>
@@ -2724,7 +2747,7 @@
       <c r="AA23" s="11"/>
     </row>
     <row r="24" spans="2:27" ht="29" customHeight="1">
-      <c r="B24" s="37">
+      <c r="B24" s="36">
         <f t="shared" si="0"/>
         <v>0.68750000000000011</v>
       </c>
@@ -2740,15 +2763,15 @@
       <c r="H24" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="I24" s="43" t="s">
-        <v>39</v>
-      </c>
-      <c r="K24" s="37">
+      <c r="I24" s="42" t="s">
+        <v>36</v>
+      </c>
+      <c r="K24" s="36">
         <f t="shared" si="1"/>
         <v>0.68750000000000011</v>
       </c>
-      <c r="L24" s="16" t="s">
-        <v>29</v>
+      <c r="L24" s="20" t="s">
+        <v>16</v>
       </c>
       <c r="M24" s="20" t="s">
         <v>16</v>
@@ -2762,11 +2785,11 @@
         <v>16</v>
       </c>
       <c r="R24" s="19"/>
-      <c r="T24" s="37">
+      <c r="T24" s="36">
         <f t="shared" si="2"/>
         <v>0.68750000000000011</v>
       </c>
-      <c r="U24" s="39"/>
+      <c r="U24" s="38"/>
       <c r="V24" s="20" t="s">
         <v>16</v>
       </c>
@@ -2777,7 +2800,7 @@
       <c r="AA24" s="19"/>
     </row>
     <row r="25" spans="2:27" ht="29" customHeight="1">
-      <c r="B25" s="37">
+      <c r="B25" s="36">
         <f t="shared" si="0"/>
         <v>0.70833333333333348</v>
       </c>
@@ -2791,15 +2814,15 @@
       <c r="H25" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="I25" s="43" t="s">
-        <v>39</v>
-      </c>
-      <c r="K25" s="37">
+      <c r="I25" s="42" t="s">
+        <v>36</v>
+      </c>
+      <c r="K25" s="36">
         <f t="shared" si="1"/>
         <v>0.70833333333333348</v>
       </c>
-      <c r="L25" s="16" t="s">
-        <v>29</v>
+      <c r="L25" s="20" t="s">
+        <v>16</v>
       </c>
       <c r="M25" s="20" t="s">
         <v>16</v>
@@ -2815,11 +2838,11 @@
         <v>16</v>
       </c>
       <c r="R25" s="19"/>
-      <c r="T25" s="37">
+      <c r="T25" s="36">
         <f t="shared" si="2"/>
         <v>0.70833333333333348</v>
       </c>
-      <c r="U25" s="32"/>
+      <c r="U25" s="31"/>
       <c r="V25" s="20" t="s">
         <v>16</v>
       </c>
@@ -2836,7 +2859,7 @@
       </c>
     </row>
     <row r="26" spans="2:27" ht="29" customHeight="1">
-      <c r="B26" s="37">
+      <c r="B26" s="36">
         <f t="shared" si="0"/>
         <v>0.72916666666666685</v>
       </c>
@@ -2851,23 +2874,25 @@
         <v>16</v>
       </c>
       <c r="G26" s="20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H26" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="I26" s="43" t="s">
-        <v>39</v>
-      </c>
-      <c r="K26" s="37">
+      <c r="I26" s="42" t="s">
+        <v>36</v>
+      </c>
+      <c r="K26" s="36">
         <f t="shared" si="1"/>
         <v>0.72916666666666685</v>
       </c>
-      <c r="L26" s="24"/>
+      <c r="L26" s="20" t="s">
+        <v>16</v>
+      </c>
       <c r="M26" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="N26" s="40"/>
+      <c r="N26" s="39"/>
       <c r="O26" s="20" t="s">
         <v>16</v>
       </c>
@@ -2880,7 +2905,7 @@
       <c r="R26" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="T26" s="37">
+      <c r="T26" s="36">
         <f t="shared" si="2"/>
         <v>0.72916666666666685</v>
       </c>
@@ -2888,7 +2913,7 @@
       <c r="V26" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="W26" s="40"/>
+      <c r="W26" s="39"/>
       <c r="X26" s="20" t="s">
         <v>16</v>
       </c>
@@ -2903,7 +2928,7 @@
       </c>
     </row>
     <row r="27" spans="2:27" ht="29" customHeight="1">
-      <c r="B27" s="37">
+      <c r="B27" s="36">
         <f t="shared" si="0"/>
         <v>0.75000000000000022</v>
       </c>
@@ -2918,13 +2943,13 @@
         <v>16</v>
       </c>
       <c r="G27" s="20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H27" s="18"/>
-      <c r="I27" s="42" t="s">
-        <v>38</v>
-      </c>
-      <c r="K27" s="37">
+      <c r="I27" s="41" t="s">
+        <v>35</v>
+      </c>
+      <c r="K27" s="36">
         <f t="shared" si="1"/>
         <v>0.75000000000000022</v>
       </c>
@@ -2943,7 +2968,7 @@
       <c r="R27" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="T27" s="37">
+      <c r="T27" s="36">
         <f t="shared" si="2"/>
         <v>0.75000000000000022</v>
       </c>
@@ -2966,7 +2991,7 @@
       </c>
     </row>
     <row r="28" spans="2:27" ht="29" customHeight="1">
-      <c r="B28" s="37">
+      <c r="B28" s="36">
         <f t="shared" si="0"/>
         <v>0.77083333333333359</v>
       </c>
@@ -2982,10 +3007,10 @@
       <c r="F28" s="18"/>
       <c r="G28" s="28"/>
       <c r="H28" s="18"/>
-      <c r="I28" s="42" t="s">
-        <v>38</v>
-      </c>
-      <c r="K28" s="37">
+      <c r="I28" s="41" t="s">
+        <v>35</v>
+      </c>
+      <c r="K28" s="36">
         <f t="shared" si="1"/>
         <v>0.77083333333333359</v>
       </c>
@@ -3006,7 +3031,7 @@
       <c r="R28" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="T28" s="37">
+      <c r="T28" s="36">
         <f t="shared" si="2"/>
         <v>0.77083333333333359</v>
       </c>
@@ -3029,7 +3054,7 @@
       </c>
     </row>
     <row r="29" spans="2:27" ht="29" customHeight="1">
-      <c r="B29" s="37">
+      <c r="B29" s="36">
         <f t="shared" si="0"/>
         <v>0.79166666666666696</v>
       </c>
@@ -3041,14 +3066,14 @@
         <v>16</v>
       </c>
       <c r="F29" s="22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G29" s="28"/>
       <c r="H29" s="18"/>
-      <c r="I29" s="42" t="s">
-        <v>38</v>
-      </c>
-      <c r="K29" s="37">
+      <c r="I29" s="41" t="s">
+        <v>35</v>
+      </c>
+      <c r="K29" s="36">
         <f t="shared" si="1"/>
         <v>0.79166666666666696</v>
       </c>
@@ -3069,12 +3094,12 @@
       <c r="R29" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="T29" s="37">
+      <c r="T29" s="36">
         <f t="shared" si="2"/>
         <v>0.79166666666666696</v>
       </c>
       <c r="U29" s="16" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="V29" s="20" t="s">
         <v>16</v>
@@ -3096,7 +3121,7 @@
       </c>
     </row>
     <row r="30" spans="2:27" ht="29" customHeight="1">
-      <c r="B30" s="37">
+      <c r="B30" s="36">
         <f t="shared" si="0"/>
         <v>0.81250000000000033</v>
       </c>
@@ -3104,7 +3129,7 @@
         <v>13</v>
       </c>
       <c r="D30" s="22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E30" s="20" t="s">
         <v>16</v>
@@ -3112,18 +3137,16 @@
       <c r="F30" s="24"/>
       <c r="G30" s="28"/>
       <c r="H30" s="18"/>
-      <c r="I30" s="42" t="s">
-        <v>38</v>
-      </c>
-      <c r="K30" s="37">
+      <c r="I30" s="41" t="s">
+        <v>35</v>
+      </c>
+      <c r="K30" s="36">
         <f t="shared" si="1"/>
         <v>0.81250000000000033</v>
       </c>
       <c r="L30" s="27"/>
       <c r="M30" s="24"/>
-      <c r="N30" s="20" t="s">
-        <v>16</v>
-      </c>
+      <c r="N30" s="39"/>
       <c r="O30" s="20" t="s">
         <v>16</v>
       </c>
@@ -3136,12 +3159,12 @@
       <c r="R30" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="T30" s="37">
+      <c r="T30" s="36">
         <f t="shared" si="2"/>
         <v>0.81250000000000033</v>
       </c>
       <c r="U30" s="16" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="V30" s="20" t="s">
         <v>16</v>
@@ -3163,32 +3186,30 @@
       </c>
     </row>
     <row r="31" spans="2:27" ht="29" customHeight="1">
-      <c r="B31" s="37">
+      <c r="B31" s="36">
         <f t="shared" si="0"/>
         <v>0.8333333333333337</v>
       </c>
       <c r="C31" s="19"/>
       <c r="D31" s="22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E31" s="18"/>
       <c r="F31" s="22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G31" s="28"/>
       <c r="H31" s="18"/>
-      <c r="I31" s="42" t="s">
-        <v>38</v>
-      </c>
-      <c r="K31" s="37">
+      <c r="I31" s="41" t="s">
+        <v>35</v>
+      </c>
+      <c r="K31" s="36">
         <f t="shared" si="1"/>
         <v>0.8333333333333337</v>
       </c>
-      <c r="L31" s="40"/>
+      <c r="L31" s="39"/>
       <c r="M31" s="24"/>
-      <c r="N31" s="20" t="s">
-        <v>16</v>
-      </c>
+      <c r="N31" s="39"/>
       <c r="O31" s="20" t="s">
         <v>16</v>
       </c>
@@ -3201,12 +3222,12 @@
       <c r="R31" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="T31" s="37">
+      <c r="T31" s="36">
         <f t="shared" si="2"/>
         <v>0.8333333333333337</v>
       </c>
       <c r="U31" s="16" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="V31" s="20" t="s">
         <v>16</v>
@@ -3228,7 +3249,7 @@
       </c>
     </row>
     <row r="32" spans="2:27" ht="29" customHeight="1">
-      <c r="B32" s="37">
+      <c r="B32" s="36">
         <f t="shared" si="0"/>
         <v>0.85416666666666707</v>
       </c>
@@ -3236,28 +3257,26 @@
         <v>13</v>
       </c>
       <c r="D32" s="22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E32" s="22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F32" s="22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G32" s="18"/>
       <c r="H32" s="18"/>
-      <c r="I32" s="42" t="s">
-        <v>38</v>
-      </c>
-      <c r="K32" s="37">
+      <c r="I32" s="41" t="s">
+        <v>35</v>
+      </c>
+      <c r="K32" s="36">
         <f t="shared" si="1"/>
         <v>0.85416666666666707</v>
       </c>
       <c r="L32" s="27"/>
       <c r="M32" s="24"/>
-      <c r="N32" s="20" t="s">
-        <v>16</v>
-      </c>
+      <c r="N32" s="39"/>
       <c r="O32" s="20" t="s">
         <v>16</v>
       </c>
@@ -3270,12 +3289,12 @@
       <c r="R32" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="T32" s="37">
+      <c r="T32" s="36">
         <f t="shared" si="2"/>
         <v>0.85416666666666707</v>
       </c>
       <c r="U32" s="16" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="V32" s="20" t="s">
         <v>16</v>
@@ -3297,7 +3316,7 @@
       </c>
     </row>
     <row r="33" spans="2:27" ht="29" customHeight="1">
-      <c r="B33" s="37">
+      <c r="B33" s="36">
         <f t="shared" si="0"/>
         <v>0.87500000000000044</v>
       </c>
@@ -3305,13 +3324,13 @@
         <v>13</v>
       </c>
       <c r="D33" s="22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E33" s="22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F33" s="22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G33" s="20" t="s">
         <v>14</v>
@@ -3320,15 +3339,13 @@
       <c r="I33" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="K33" s="37">
+      <c r="K33" s="36">
         <f t="shared" si="1"/>
         <v>0.87500000000000044</v>
       </c>
       <c r="L33" s="27"/>
       <c r="M33" s="24"/>
-      <c r="N33" s="20" t="s">
-        <v>16</v>
-      </c>
+      <c r="N33" s="39"/>
       <c r="O33" s="20" t="s">
         <v>16</v>
       </c>
@@ -3341,12 +3358,12 @@
       <c r="R33" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="T33" s="37">
+      <c r="T33" s="36">
         <f t="shared" si="2"/>
         <v>0.87500000000000044</v>
       </c>
       <c r="U33" s="16" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="V33" s="20" t="s">
         <v>16</v>
@@ -3368,7 +3385,7 @@
       </c>
     </row>
     <row r="34" spans="2:27" ht="29" customHeight="1">
-      <c r="B34" s="37">
+      <c r="B34" s="36">
         <f t="shared" si="0"/>
         <v>0.89583333333333381</v>
       </c>
@@ -3376,13 +3393,13 @@
         <v>13</v>
       </c>
       <c r="D34" s="22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E34" s="22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F34" s="22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G34" s="20" t="s">
         <v>15</v>
@@ -3391,15 +3408,13 @@
       <c r="I34" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="K34" s="37">
+      <c r="K34" s="36">
         <f t="shared" si="1"/>
         <v>0.89583333333333381</v>
       </c>
       <c r="L34" s="27"/>
       <c r="M34" s="24"/>
-      <c r="N34" s="20" t="s">
-        <v>16</v>
-      </c>
+      <c r="N34" s="39"/>
       <c r="O34" s="20" t="s">
         <v>16</v>
       </c>
@@ -3412,12 +3427,12 @@
       <c r="R34" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="T34" s="37">
+      <c r="T34" s="36">
         <f t="shared" si="2"/>
         <v>0.89583333333333381</v>
       </c>
       <c r="U34" s="16" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="V34" s="20" t="s">
         <v>16</v>
@@ -3439,19 +3454,19 @@
       </c>
     </row>
     <row r="35" spans="2:27" ht="29" customHeight="1">
-      <c r="B35" s="37">
+      <c r="B35" s="36">
         <f t="shared" si="0"/>
         <v>0.91666666666666718</v>
       </c>
       <c r="C35" s="18"/>
       <c r="D35" s="22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E35" s="22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F35" s="22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G35" s="20" t="s">
         <v>16</v>
@@ -3460,15 +3475,13 @@
       <c r="I35" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="K35" s="37">
+      <c r="K35" s="36">
         <f t="shared" si="1"/>
         <v>0.91666666666666718</v>
       </c>
       <c r="L35" s="28"/>
-      <c r="M35" s="32"/>
-      <c r="N35" s="20" t="s">
-        <v>16</v>
-      </c>
+      <c r="M35" s="31"/>
+      <c r="N35" s="39"/>
       <c r="O35" s="24"/>
       <c r="P35" s="19"/>
       <c r="Q35" s="20" t="s">
@@ -3477,12 +3490,12 @@
       <c r="R35" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="T35" s="37">
+      <c r="T35" s="36">
         <f t="shared" si="2"/>
         <v>0.91666666666666718</v>
       </c>
       <c r="U35" s="16" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="V35" s="20" t="s">
         <v>16</v>
@@ -3504,7 +3517,7 @@
       </c>
     </row>
     <row r="36" spans="2:27" ht="29" customHeight="1">
-      <c r="B36" s="37">
+      <c r="B36" s="36">
         <f t="shared" si="0"/>
         <v>0.93750000000000056</v>
       </c>
@@ -3512,13 +3525,13 @@
         <v>14</v>
       </c>
       <c r="D36" s="22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E36" s="22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F36" s="22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G36" s="20" t="s">
         <v>16</v>
@@ -3527,13 +3540,15 @@
       <c r="I36" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="K36" s="37">
+      <c r="K36" s="36">
         <f t="shared" si="1"/>
         <v>0.93750000000000056</v>
       </c>
-      <c r="L36" s="40"/>
+      <c r="L36" s="39"/>
       <c r="M36" s="19"/>
-      <c r="N36" s="24"/>
+      <c r="N36" s="20" t="s">
+        <v>16</v>
+      </c>
       <c r="O36" s="24"/>
       <c r="P36" s="19"/>
       <c r="Q36" s="20" t="s">
@@ -3542,12 +3557,12 @@
       <c r="R36" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="T36" s="37">
+      <c r="T36" s="36">
         <f t="shared" si="2"/>
         <v>0.93750000000000056</v>
       </c>
       <c r="U36" s="16" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="V36" s="20" t="s">
         <v>16</v>
@@ -3569,7 +3584,7 @@
       </c>
     </row>
     <row r="37" spans="2:27" ht="29" customHeight="1">
-      <c r="B37" s="37">
+      <c r="B37" s="36">
         <f t="shared" si="0"/>
         <v>0.95833333333333393</v>
       </c>
@@ -3581,7 +3596,7 @@
       </c>
       <c r="E37" s="18"/>
       <c r="F37" s="22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G37" s="20" t="s">
         <v>16</v>
@@ -3590,23 +3605,25 @@
       <c r="I37" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="K37" s="37">
+      <c r="K37" s="36">
         <f t="shared" si="1"/>
         <v>0.95833333333333393</v>
       </c>
-      <c r="L37" s="40"/>
+      <c r="L37" s="39"/>
       <c r="M37" s="19"/>
-      <c r="N37" s="32"/>
-      <c r="O37" s="32"/>
+      <c r="N37" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="O37" s="31"/>
       <c r="P37" s="19"/>
-      <c r="Q37" s="32"/>
-      <c r="R37" s="32"/>
-      <c r="T37" s="37">
+      <c r="Q37" s="31"/>
+      <c r="R37" s="31"/>
+      <c r="T37" s="36">
         <f t="shared" si="2"/>
         <v>0.95833333333333393</v>
       </c>
       <c r="U37" s="16" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="V37" s="20" t="s">
         <v>16</v>
@@ -3628,7 +3645,7 @@
       </c>
     </row>
     <row r="38" spans="2:27" ht="29" customHeight="1">
-      <c r="B38" s="37">
+      <c r="B38" s="36">
         <f t="shared" si="0"/>
         <v>0.9791666666666673</v>
       </c>
@@ -3642,7 +3659,7 @@
         <v>13</v>
       </c>
       <c r="F38" s="22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G38" s="20" t="s">
         <v>16</v>
@@ -3651,23 +3668,25 @@
       <c r="I38" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="K38" s="37">
+      <c r="K38" s="36">
         <f t="shared" si="1"/>
         <v>0.9791666666666673</v>
       </c>
-      <c r="L38" s="40"/>
+      <c r="L38" s="39"/>
       <c r="M38" s="19"/>
-      <c r="N38" s="24"/>
-      <c r="O38" s="32"/>
-      <c r="P38" s="32"/>
-      <c r="Q38" s="32"/>
-      <c r="R38" s="32"/>
-      <c r="T38" s="37">
+      <c r="N38" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="O38" s="31"/>
+      <c r="P38" s="31"/>
+      <c r="Q38" s="31"/>
+      <c r="R38" s="31"/>
+      <c r="T38" s="36">
         <f t="shared" si="2"/>
         <v>0.9791666666666673</v>
       </c>
       <c r="U38" s="16" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="V38" s="20" t="s">
         <v>16</v>
@@ -3689,7 +3708,7 @@
       </c>
     </row>
     <row r="39" spans="2:27" ht="29" customHeight="1">
-      <c r="B39" s="37">
+      <c r="B39" s="36">
         <f t="shared" ref="B39:B52" si="3">B38+TIME(0,30,0)</f>
         <v>1.0000000000000007</v>
       </c>
@@ -3703,7 +3722,7 @@
         <v>13</v>
       </c>
       <c r="F39" s="22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G39" s="20" t="s">
         <v>16</v>
@@ -3712,23 +3731,25 @@
       <c r="I39" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="K39" s="37">
+      <c r="K39" s="36">
         <f t="shared" si="1"/>
         <v>1.0000000000000007</v>
       </c>
-      <c r="L39" s="40"/>
+      <c r="L39" s="39"/>
       <c r="M39" s="19"/>
-      <c r="N39" s="24"/>
-      <c r="O39" s="32"/>
-      <c r="P39" s="32"/>
-      <c r="Q39" s="32"/>
-      <c r="R39" s="32"/>
-      <c r="T39" s="37">
+      <c r="N39" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="O39" s="31"/>
+      <c r="P39" s="31"/>
+      <c r="Q39" s="31"/>
+      <c r="R39" s="31"/>
+      <c r="T39" s="36">
         <f t="shared" si="2"/>
         <v>1.0000000000000007</v>
       </c>
       <c r="U39" s="16" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="V39" s="20" t="s">
         <v>16</v>
@@ -3750,7 +3771,7 @@
       </c>
     </row>
     <row r="40" spans="2:27" ht="29" customHeight="1">
-      <c r="B40" s="37">
+      <c r="B40" s="36">
         <f t="shared" si="3"/>
         <v>1.0208333333333339</v>
       </c>
@@ -3764,38 +3785,40 @@
         <v>13</v>
       </c>
       <c r="F40" s="22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G40" s="20" t="s">
         <v>16</v>
       </c>
       <c r="H40" s="18"/>
-      <c r="I40" s="32"/>
-      <c r="K40" s="37">
+      <c r="I40" s="31"/>
+      <c r="K40" s="36">
         <f t="shared" si="1"/>
         <v>1.0208333333333339</v>
       </c>
-      <c r="L40" s="40"/>
+      <c r="L40" s="39"/>
       <c r="M40" s="19"/>
-      <c r="N40" s="24"/>
-      <c r="O40" s="32"/>
-      <c r="P40" s="32"/>
-      <c r="Q40" s="32"/>
-      <c r="R40" s="32"/>
-      <c r="T40" s="37">
+      <c r="N40" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="O40" s="31"/>
+      <c r="P40" s="31"/>
+      <c r="Q40" s="31"/>
+      <c r="R40" s="31"/>
+      <c r="T40" s="36">
         <f t="shared" si="2"/>
         <v>1.0208333333333339</v>
       </c>
       <c r="U40" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="V40" s="41" t="s">
-        <v>16</v>
-      </c>
-      <c r="W40" s="41" t="s">
-        <v>16</v>
-      </c>
-      <c r="X40" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="V40" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="W40" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="X40" s="40" t="s">
         <v>16</v>
       </c>
       <c r="Y40" s="20" t="s">
@@ -3804,12 +3827,12 @@
       <c r="Z40" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="AA40" s="41" t="s">
+      <c r="AA40" s="40" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="41" spans="2:27" ht="29" customHeight="1">
-      <c r="B41" s="37">
+      <c r="B41" s="36">
         <f t="shared" si="3"/>
         <v>1.0416666666666672</v>
       </c>
@@ -3817,38 +3840,40 @@
       <c r="D41" s="18"/>
       <c r="E41" s="18"/>
       <c r="F41" s="22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G41" s="18"/>
       <c r="H41" s="18"/>
-      <c r="I41" s="32"/>
-      <c r="K41" s="37">
+      <c r="I41" s="31"/>
+      <c r="K41" s="36">
         <f t="shared" si="1"/>
         <v>1.0416666666666672</v>
       </c>
       <c r="L41" s="28"/>
-      <c r="M41" s="32"/>
-      <c r="N41" s="32"/>
-      <c r="O41" s="32"/>
-      <c r="P41" s="32"/>
-      <c r="Q41" s="32"/>
-      <c r="R41" s="32"/>
-      <c r="T41" s="37">
+      <c r="M41" s="31"/>
+      <c r="N41" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="O41" s="31"/>
+      <c r="P41" s="31"/>
+      <c r="Q41" s="31"/>
+      <c r="R41" s="31"/>
+      <c r="T41" s="36">
         <f t="shared" si="2"/>
         <v>1.0416666666666672</v>
       </c>
       <c r="U41" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="V41" s="32"/>
-      <c r="W41" s="32"/>
-      <c r="X41" s="32"/>
-      <c r="Y41" s="32"/>
-      <c r="Z41" s="32"/>
-      <c r="AA41" s="32"/>
+        <v>32</v>
+      </c>
+      <c r="V41" s="31"/>
+      <c r="W41" s="31"/>
+      <c r="X41" s="31"/>
+      <c r="Y41" s="31"/>
+      <c r="Z41" s="31"/>
+      <c r="AA41" s="31"/>
     </row>
     <row r="42" spans="2:27" ht="29" customHeight="1">
-      <c r="B42" s="37">
+      <c r="B42" s="36">
         <f t="shared" si="3"/>
         <v>1.0625000000000004</v>
       </c>
@@ -3856,28 +3881,28 @@
       <c r="D42" s="18"/>
       <c r="E42" s="18"/>
       <c r="F42" s="22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G42" s="18"/>
       <c r="H42" s="18"/>
       <c r="I42" s="18"/>
-      <c r="K42" s="37">
+      <c r="K42" s="36">
         <f t="shared" si="1"/>
         <v>1.0625000000000004</v>
       </c>
-      <c r="L42" s="32"/>
-      <c r="M42" s="32"/>
-      <c r="N42" s="32"/>
-      <c r="O42" s="32"/>
-      <c r="P42" s="32"/>
-      <c r="Q42" s="32"/>
-      <c r="R42" s="32"/>
-      <c r="T42" s="37">
+      <c r="L42" s="31"/>
+      <c r="M42" s="31"/>
+      <c r="N42" s="31"/>
+      <c r="O42" s="31"/>
+      <c r="P42" s="31"/>
+      <c r="Q42" s="31"/>
+      <c r="R42" s="31"/>
+      <c r="T42" s="36">
         <f t="shared" si="2"/>
         <v>1.0625000000000004</v>
       </c>
       <c r="U42" s="16" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="V42" s="18"/>
       <c r="W42" s="18"/>
@@ -3887,7 +3912,7 @@
       <c r="AA42" s="18"/>
     </row>
     <row r="43" spans="2:27" ht="29" customHeight="1">
-      <c r="B43" s="37">
+      <c r="B43" s="36">
         <f t="shared" si="3"/>
         <v>1.0833333333333337</v>
       </c>
@@ -3898,23 +3923,23 @@
       <c r="G43" s="18"/>
       <c r="H43" s="18"/>
       <c r="I43" s="18"/>
-      <c r="K43" s="37">
+      <c r="K43" s="36">
         <f t="shared" si="1"/>
         <v>1.0833333333333337</v>
       </c>
-      <c r="L43" s="32"/>
-      <c r="M43" s="32"/>
-      <c r="N43" s="32"/>
-      <c r="O43" s="32"/>
-      <c r="P43" s="32"/>
-      <c r="Q43" s="32"/>
-      <c r="R43" s="32"/>
-      <c r="T43" s="37">
+      <c r="L43" s="31"/>
+      <c r="M43" s="31"/>
+      <c r="N43" s="31"/>
+      <c r="O43" s="31"/>
+      <c r="P43" s="31"/>
+      <c r="Q43" s="31"/>
+      <c r="R43" s="31"/>
+      <c r="T43" s="36">
         <f t="shared" si="2"/>
         <v>1.0833333333333337</v>
       </c>
       <c r="U43" s="16" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="V43" s="18"/>
       <c r="W43" s="18"/>
@@ -3924,7 +3949,7 @@
       <c r="AA43" s="18"/>
     </row>
     <row r="44" spans="2:27" ht="29" customHeight="1">
-      <c r="B44" s="37">
+      <c r="B44" s="36">
         <f t="shared" si="3"/>
         <v>1.104166666666667</v>
       </c>
@@ -3935,23 +3960,23 @@
       <c r="G44" s="18"/>
       <c r="H44" s="18"/>
       <c r="I44" s="18"/>
-      <c r="K44" s="37">
+      <c r="K44" s="36">
         <f t="shared" si="1"/>
         <v>1.104166666666667</v>
       </c>
-      <c r="L44" s="32"/>
-      <c r="M44" s="32"/>
-      <c r="N44" s="32"/>
-      <c r="O44" s="32"/>
-      <c r="P44" s="32"/>
-      <c r="Q44" s="32"/>
-      <c r="R44" s="32"/>
-      <c r="T44" s="37">
+      <c r="L44" s="31"/>
+      <c r="M44" s="31"/>
+      <c r="N44" s="31"/>
+      <c r="O44" s="31"/>
+      <c r="P44" s="31"/>
+      <c r="Q44" s="31"/>
+      <c r="R44" s="31"/>
+      <c r="T44" s="36">
         <f t="shared" si="2"/>
         <v>1.104166666666667</v>
       </c>
       <c r="U44" s="16" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="V44" s="18"/>
       <c r="W44" s="18"/>
@@ -3961,7 +3986,7 @@
       <c r="AA44" s="18"/>
     </row>
     <row r="45" spans="2:27" ht="29" customHeight="1">
-      <c r="B45" s="37">
+      <c r="B45" s="36">
         <f t="shared" si="3"/>
         <v>1.1250000000000002</v>
       </c>
@@ -3972,23 +3997,23 @@
       <c r="G45" s="18"/>
       <c r="H45" s="18"/>
       <c r="I45" s="18"/>
-      <c r="K45" s="37">
+      <c r="K45" s="36">
         <f t="shared" si="1"/>
         <v>1.1250000000000002</v>
       </c>
-      <c r="L45" s="32"/>
-      <c r="M45" s="32"/>
-      <c r="N45" s="32"/>
-      <c r="O45" s="32"/>
-      <c r="P45" s="32"/>
-      <c r="Q45" s="32"/>
-      <c r="R45" s="32"/>
-      <c r="T45" s="37">
+      <c r="L45" s="31"/>
+      <c r="M45" s="31"/>
+      <c r="N45" s="31"/>
+      <c r="O45" s="31"/>
+      <c r="P45" s="31"/>
+      <c r="Q45" s="31"/>
+      <c r="R45" s="31"/>
+      <c r="T45" s="36">
         <f t="shared" si="2"/>
         <v>1.1250000000000002</v>
       </c>
       <c r="U45" s="16" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="V45" s="18"/>
       <c r="W45" s="18"/>
@@ -3998,7 +4023,7 @@
       <c r="AA45" s="18"/>
     </row>
     <row r="46" spans="2:27" ht="29" customHeight="1">
-      <c r="B46" s="37">
+      <c r="B46" s="36">
         <f t="shared" si="3"/>
         <v>1.1458333333333335</v>
       </c>
@@ -4009,23 +4034,23 @@
       <c r="G46" s="18"/>
       <c r="H46" s="18"/>
       <c r="I46" s="18"/>
-      <c r="K46" s="37">
+      <c r="K46" s="36">
         <f t="shared" si="1"/>
         <v>1.1458333333333335</v>
       </c>
-      <c r="L46" s="32"/>
-      <c r="M46" s="32"/>
-      <c r="N46" s="32"/>
-      <c r="O46" s="32"/>
-      <c r="P46" s="32"/>
-      <c r="Q46" s="32"/>
-      <c r="R46" s="32"/>
-      <c r="T46" s="37">
+      <c r="L46" s="31"/>
+      <c r="M46" s="31"/>
+      <c r="N46" s="31"/>
+      <c r="O46" s="31"/>
+      <c r="P46" s="31"/>
+      <c r="Q46" s="31"/>
+      <c r="R46" s="31"/>
+      <c r="T46" s="36">
         <f t="shared" si="2"/>
         <v>1.1458333333333335</v>
       </c>
       <c r="U46" s="16" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="V46" s="18"/>
       <c r="W46" s="18"/>
@@ -4035,7 +4060,7 @@
       <c r="AA46" s="18"/>
     </row>
     <row r="47" spans="2:27" ht="29" customHeight="1">
-      <c r="B47" s="37">
+      <c r="B47" s="36">
         <f t="shared" si="3"/>
         <v>1.1666666666666667</v>
       </c>
@@ -4046,18 +4071,18 @@
       <c r="G47" s="18"/>
       <c r="H47" s="18"/>
       <c r="I47" s="18"/>
-      <c r="K47" s="37">
+      <c r="K47" s="36">
         <f t="shared" si="1"/>
         <v>1.1666666666666667</v>
       </c>
-      <c r="L47" s="32"/>
-      <c r="M47" s="32"/>
-      <c r="N47" s="32"/>
-      <c r="O47" s="32"/>
-      <c r="P47" s="32"/>
-      <c r="Q47" s="32"/>
-      <c r="R47" s="32"/>
-      <c r="T47" s="37">
+      <c r="L47" s="31"/>
+      <c r="M47" s="31"/>
+      <c r="N47" s="31"/>
+      <c r="O47" s="31"/>
+      <c r="P47" s="31"/>
+      <c r="Q47" s="31"/>
+      <c r="R47" s="31"/>
+      <c r="T47" s="36">
         <f t="shared" si="2"/>
         <v>1.1666666666666667</v>
       </c>
@@ -4070,7 +4095,7 @@
       <c r="AA47" s="18"/>
     </row>
     <row r="48" spans="2:27" ht="29" customHeight="1">
-      <c r="B48" s="37">
+      <c r="B48" s="36">
         <f t="shared" si="3"/>
         <v>1.1875</v>
       </c>
@@ -4081,18 +4106,18 @@
       <c r="G48" s="18"/>
       <c r="H48" s="18"/>
       <c r="I48" s="18"/>
-      <c r="K48" s="37">
+      <c r="K48" s="36">
         <f t="shared" si="1"/>
         <v>1.1875</v>
       </c>
-      <c r="L48" s="32"/>
-      <c r="M48" s="32"/>
-      <c r="N48" s="32"/>
-      <c r="O48" s="32"/>
-      <c r="P48" s="32"/>
-      <c r="Q48" s="32"/>
-      <c r="R48" s="32"/>
-      <c r="T48" s="37">
+      <c r="L48" s="31"/>
+      <c r="M48" s="31"/>
+      <c r="N48" s="31"/>
+      <c r="O48" s="31"/>
+      <c r="P48" s="31"/>
+      <c r="Q48" s="31"/>
+      <c r="R48" s="31"/>
+      <c r="T48" s="36">
         <f t="shared" si="2"/>
         <v>1.1875</v>
       </c>
@@ -4105,7 +4130,7 @@
       <c r="AA48" s="18"/>
     </row>
     <row r="49" spans="2:27" ht="29" customHeight="1">
-      <c r="B49" s="37">
+      <c r="B49" s="36">
         <f t="shared" si="3"/>
         <v>1.2083333333333333</v>
       </c>
@@ -4116,18 +4141,18 @@
       <c r="G49" s="18"/>
       <c r="H49" s="18"/>
       <c r="I49" s="18"/>
-      <c r="K49" s="37">
+      <c r="K49" s="36">
         <f t="shared" si="1"/>
         <v>1.2083333333333333</v>
       </c>
-      <c r="L49" s="32"/>
-      <c r="M49" s="32"/>
-      <c r="N49" s="32"/>
-      <c r="O49" s="32"/>
-      <c r="P49" s="32"/>
-      <c r="Q49" s="32"/>
-      <c r="R49" s="32"/>
-      <c r="T49" s="37">
+      <c r="L49" s="31"/>
+      <c r="M49" s="31"/>
+      <c r="N49" s="31"/>
+      <c r="O49" s="31"/>
+      <c r="P49" s="31"/>
+      <c r="Q49" s="31"/>
+      <c r="R49" s="31"/>
+      <c r="T49" s="36">
         <f t="shared" si="2"/>
         <v>1.2083333333333333</v>
       </c>
@@ -4140,7 +4165,7 @@
       <c r="AA49" s="18"/>
     </row>
     <row r="50" spans="2:27" ht="29" customHeight="1">
-      <c r="B50" s="37">
+      <c r="B50" s="36">
         <f t="shared" si="3"/>
         <v>1.2291666666666665</v>
       </c>
@@ -4151,18 +4176,18 @@
       <c r="G50" s="18"/>
       <c r="H50" s="18"/>
       <c r="I50" s="18"/>
-      <c r="K50" s="37">
+      <c r="K50" s="36">
         <f t="shared" si="1"/>
         <v>1.2291666666666665</v>
       </c>
-      <c r="L50" s="32"/>
-      <c r="M50" s="32"/>
-      <c r="N50" s="32"/>
-      <c r="O50" s="32"/>
-      <c r="P50" s="32"/>
-      <c r="Q50" s="32"/>
-      <c r="R50" s="32"/>
-      <c r="T50" s="37">
+      <c r="L50" s="31"/>
+      <c r="M50" s="31"/>
+      <c r="N50" s="31"/>
+      <c r="O50" s="31"/>
+      <c r="P50" s="31"/>
+      <c r="Q50" s="31"/>
+      <c r="R50" s="31"/>
+      <c r="T50" s="36">
         <f t="shared" si="2"/>
         <v>1.2291666666666665</v>
       </c>
@@ -4175,7 +4200,7 @@
       <c r="AA50" s="18"/>
     </row>
     <row r="51" spans="2:27" ht="29" customHeight="1">
-      <c r="B51" s="37">
+      <c r="B51" s="36">
         <f t="shared" si="3"/>
         <v>1.2499999999999998</v>
       </c>
@@ -4186,18 +4211,18 @@
       <c r="G51" s="18"/>
       <c r="H51" s="18"/>
       <c r="I51" s="18"/>
-      <c r="K51" s="37">
+      <c r="K51" s="36">
         <f t="shared" si="1"/>
         <v>1.2499999999999998</v>
       </c>
-      <c r="L51" s="32"/>
-      <c r="M51" s="32"/>
-      <c r="N51" s="32"/>
-      <c r="O51" s="32"/>
-      <c r="P51" s="32"/>
-      <c r="Q51" s="32"/>
-      <c r="R51" s="32"/>
-      <c r="T51" s="37">
+      <c r="L51" s="31"/>
+      <c r="M51" s="31"/>
+      <c r="N51" s="31"/>
+      <c r="O51" s="31"/>
+      <c r="P51" s="31"/>
+      <c r="Q51" s="31"/>
+      <c r="R51" s="31"/>
+      <c r="T51" s="36">
         <f t="shared" si="2"/>
         <v>1.2499999999999998</v>
       </c>
@@ -4210,7 +4235,7 @@
       <c r="AA51" s="18"/>
     </row>
     <row r="52" spans="2:27" ht="29" customHeight="1">
-      <c r="B52" s="37">
+      <c r="B52" s="36">
         <f t="shared" si="3"/>
         <v>1.270833333333333</v>
       </c>
@@ -4221,18 +4246,18 @@
       <c r="G52" s="18"/>
       <c r="H52" s="18"/>
       <c r="I52" s="18"/>
-      <c r="K52" s="37">
+      <c r="K52" s="36">
         <f t="shared" si="1"/>
         <v>1.270833333333333</v>
       </c>
-      <c r="L52" s="32"/>
-      <c r="M52" s="32"/>
-      <c r="N52" s="32"/>
-      <c r="O52" s="32"/>
-      <c r="P52" s="32"/>
-      <c r="Q52" s="32"/>
-      <c r="R52" s="32"/>
-      <c r="T52" s="37">
+      <c r="L52" s="31"/>
+      <c r="M52" s="31"/>
+      <c r="N52" s="31"/>
+      <c r="O52" s="31"/>
+      <c r="P52" s="31"/>
+      <c r="Q52" s="31"/>
+      <c r="R52" s="31"/>
+      <c r="T52" s="36">
         <f t="shared" si="2"/>
         <v>1.270833333333333</v>
       </c>

</xml_diff>

<commit_message>
Updated interview questions to match what i have been actually asking most of the time, added last weeks meeting minutes, added current state of my final report
</commit_message>
<xml_diff>
--- a/TIMETABLE_LAST_WEEKS.xlsx
+++ b/TIMETABLE_LAST_WEEKS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lavanyasajwan/Documents/University/2020/engr489/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF85AF3-EF6A-8D4C-9F98-59EBF06F6917}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2139509-6D34-D74F-AFC3-EB657F21AF9B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1481,8 +1481,8 @@
   </sheetPr>
   <dimension ref="B1:AA52"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F11" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="L26" sqref="K5:R52"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="29" customHeight="1"/>

</xml_diff>

<commit_message>
Latest report updates, added new emergent theory diagram, updated timetable
</commit_message>
<xml_diff>
--- a/TIMETABLE_LAST_WEEKS.xlsx
+++ b/TIMETABLE_LAST_WEEKS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lavanyasajwan/Documents/University/2020/engr489/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2139509-6D34-D74F-AFC3-EB657F21AF9B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5ACB5F1-6BC4-5E4D-A9E5-4C1CBEC4F197}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Schedule" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="41">
   <si>
     <t>Daily Schedule</t>
   </si>
@@ -1481,8 +1481,8 @@
   </sheetPr>
   <dimension ref="B1:AA52"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="L9" zoomScale="75" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="W9" sqref="T5:AA52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="29" customHeight="1"/>
@@ -2322,7 +2322,9 @@
         <v>16</v>
       </c>
       <c r="W16" s="31"/>
-      <c r="X16" s="11"/>
+      <c r="X16" s="20" t="s">
+        <v>16</v>
+      </c>
       <c r="Y16" s="20" t="s">
         <v>16</v>
       </c>
@@ -2387,8 +2389,8 @@
         <v>16</v>
       </c>
       <c r="W17" s="31"/>
-      <c r="X17" s="22" t="s">
-        <v>19</v>
+      <c r="X17" s="20" t="s">
+        <v>16</v>
       </c>
       <c r="Y17" s="20" t="s">
         <v>16</v>
@@ -2448,8 +2450,8 @@
         <v>16</v>
       </c>
       <c r="W18" s="31"/>
-      <c r="X18" s="22" t="s">
-        <v>19</v>
+      <c r="X18" s="20" t="s">
+        <v>16</v>
       </c>
       <c r="Y18" s="20" t="s">
         <v>16</v>
@@ -2503,7 +2505,9 @@
         <v>16</v>
       </c>
       <c r="W19" s="29"/>
-      <c r="X19" s="24"/>
+      <c r="X19" s="20" t="s">
+        <v>16</v>
+      </c>
       <c r="Y19" s="20" t="s">
         <v>16</v>
       </c>
@@ -2556,14 +2560,18 @@
         <v>16</v>
       </c>
       <c r="W20" s="29"/>
-      <c r="X20" s="24"/>
+      <c r="X20" s="20" t="s">
+        <v>16</v>
+      </c>
       <c r="Y20" s="20" t="s">
         <v>16</v>
       </c>
       <c r="Z20" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="AA20" s="38"/>
+      <c r="AA20" s="20" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="21" spans="2:27" ht="29" customHeight="1">
       <c r="B21" s="36">
@@ -2617,17 +2625,17 @@
         <v>16</v>
       </c>
       <c r="W21" s="29"/>
-      <c r="X21" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="Y21" s="23" t="s">
-        <v>17</v>
+      <c r="X21" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y21" s="20" t="s">
+        <v>16</v>
       </c>
       <c r="Z21" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="AA21" s="23" t="s">
-        <v>17</v>
+      <c r="AA21" s="20" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="2:27" ht="29" customHeight="1">
@@ -2684,17 +2692,17 @@
         <v>16</v>
       </c>
       <c r="W22" s="29"/>
-      <c r="X22" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="Y22" s="23" t="s">
-        <v>17</v>
+      <c r="X22" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y22" s="20" t="s">
+        <v>16</v>
       </c>
       <c r="Z22" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="AA22" s="23" t="s">
-        <v>17</v>
+      <c r="AA22" s="20" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="2:27" ht="29" customHeight="1">
@@ -2741,10 +2749,18 @@
         <v>16</v>
       </c>
       <c r="W23" s="29"/>
-      <c r="X23" s="19"/>
-      <c r="Y23" s="11"/>
-      <c r="Z23" s="11"/>
-      <c r="AA23" s="11"/>
+      <c r="X23" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y23" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z23" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA23" s="20" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="24" spans="2:27" ht="29" customHeight="1">
       <c r="B24" s="36">
@@ -2794,10 +2810,18 @@
         <v>16</v>
       </c>
       <c r="W24" s="29"/>
-      <c r="X24" s="19"/>
-      <c r="Y24" s="11"/>
-      <c r="Z24" s="11"/>
-      <c r="AA24" s="19"/>
+      <c r="X24" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y24" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z24" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA24" s="20" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="25" spans="2:27" ht="29" customHeight="1">
       <c r="B25" s="36">
@@ -2847,7 +2871,9 @@
         <v>16</v>
       </c>
       <c r="W25" s="28"/>
-      <c r="X25" s="19"/>
+      <c r="X25" s="20" t="s">
+        <v>16</v>
+      </c>
       <c r="Y25" s="20" t="s">
         <v>16</v>
       </c>
@@ -4086,7 +4112,9 @@
         <f t="shared" si="2"/>
         <v>1.1666666666666667</v>
       </c>
-      <c r="U47" s="24"/>
+      <c r="U47" s="16" t="s">
+        <v>32</v>
+      </c>
       <c r="V47" s="18"/>
       <c r="W47" s="18"/>
       <c r="X47" s="18"/>
@@ -4121,7 +4149,9 @@
         <f t="shared" si="2"/>
         <v>1.1875</v>
       </c>
-      <c r="U48" s="24"/>
+      <c r="U48" s="16" t="s">
+        <v>32</v>
+      </c>
       <c r="V48" s="18"/>
       <c r="W48" s="18"/>
       <c r="X48" s="18"/>
@@ -4156,7 +4186,9 @@
         <f t="shared" si="2"/>
         <v>1.2083333333333333</v>
       </c>
-      <c r="U49" s="24"/>
+      <c r="U49" s="16" t="s">
+        <v>32</v>
+      </c>
       <c r="V49" s="18"/>
       <c r="W49" s="18"/>
       <c r="X49" s="18"/>
@@ -4191,7 +4223,9 @@
         <f t="shared" si="2"/>
         <v>1.2291666666666665</v>
       </c>
-      <c r="U50" s="24"/>
+      <c r="U50" s="16" t="s">
+        <v>32</v>
+      </c>
       <c r="V50" s="18"/>
       <c r="W50" s="18"/>
       <c r="X50" s="18"/>
@@ -4226,7 +4260,9 @@
         <f t="shared" si="2"/>
         <v>1.2499999999999998</v>
       </c>
-      <c r="U51" s="24"/>
+      <c r="U51" s="16" t="s">
+        <v>32</v>
+      </c>
       <c r="V51" s="18"/>
       <c r="W51" s="18"/>
       <c r="X51" s="18"/>
@@ -4261,7 +4297,9 @@
         <f t="shared" si="2"/>
         <v>1.270833333333333</v>
       </c>
-      <c r="U52" s="24"/>
+      <c r="U52" s="16" t="s">
+        <v>32</v>
+      </c>
       <c r="V52" s="18"/>
       <c r="W52" s="18"/>
       <c r="X52" s="18"/>

</xml_diff>

<commit_message>
Latest version of report
</commit_message>
<xml_diff>
--- a/TIMETABLE_LAST_WEEKS.xlsx
+++ b/TIMETABLE_LAST_WEEKS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lavanyasajwan/Documents/University/2020/engr489/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5ACB5F1-6BC4-5E4D-A9E5-4C1CBEC4F197}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1B5C4F3-053B-0248-BADE-F773BF752BE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1481,8 +1481,8 @@
   </sheetPr>
   <dimension ref="B1:AA52"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="L9" zoomScale="75" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="W9" sqref="T5:AA52"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="L2" zoomScale="75" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="X16" sqref="X15:Y16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="29" customHeight="1"/>

</xml_diff>